<commit_message>
add click and dowload vep
</commit_message>
<xml_diff>
--- a/data/INPUT_DATOS_VEPS.xlsx
+++ b/data/INPUT_DATOS_VEPS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WNS\PycharmProjects\GenerarVepsAutonomos\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glorenzo\Python\VepsAutonomosPython\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2A39F3-40CA-441B-8232-896653EE8DBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0A2468-6D31-4D30-9873-E65181D5173E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -109,9 +109,6 @@
     <t>AUXILIAR (NO TOCAR NI MOVER)</t>
   </si>
   <si>
-    <t>Pepitos123</t>
-  </si>
-  <si>
     <t>LORENZO PATTI GIAN FRANCO</t>
   </si>
   <si>
@@ -154,9 +151,6 @@
     <t>Autonomo</t>
   </si>
   <si>
-    <t>04</t>
-  </si>
-  <si>
     <t>103: T1 Cat III Ingresos hasta $15.000</t>
   </si>
   <si>
@@ -212,6 +206,12 @@
   </si>
   <si>
     <t>1003 - Interbanking</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>xxx</t>
   </si>
 </sst>
 </file>
@@ -340,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -380,6 +380,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -665,30 +668,30 @@
   <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="34.21875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="2.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="46" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -698,7 +701,7 @@
       </c>
       <c r="D1" s="11"/>
       <c r="E1" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F1" s="12"/>
       <c r="G1" s="12"/>
@@ -707,7 +710,7 @@
       <c r="J1" s="12"/>
       <c r="K1" s="12"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -721,25 +724,25 @@
         <v>5</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="K2" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M2" s="13" t="s">
         <v>6</v>
@@ -749,58 +752,58 @@
       <c r="P2" s="14"/>
       <c r="Q2" s="14"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>20400903922</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>8</v>
       </c>
       <c r="D3" s="6">
         <v>20400903922</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>40</v>
       </c>
       <c r="H3" s="7">
         <v>2024</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="N3" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q3" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
@@ -808,17 +811,17 @@
       <c r="K4" s="8"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P4" s="7"/>
       <c r="Q4" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
@@ -826,17 +829,17 @@
       <c r="K5" s="8"/>
       <c r="M5" s="7"/>
       <c r="N5" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P5" s="7"/>
       <c r="Q5" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
@@ -847,115 +850,115 @@
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
       <c r="Q6" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
       <c r="P7" s="7"/>
       <c r="Q7" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
       <c r="P8" s="7"/>
       <c r="Q8" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
       <c r="Q9" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
       <c r="P10" s="7"/>
       <c r="Q10" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
       <c r="P11" s="7"/>
       <c r="Q11" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
       <c r="P12" s="7"/>
       <c r="Q12" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M13" s="7"/>
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
       <c r="P13" s="7"/>
       <c r="Q13" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
       <c r="P14" s="7"/>
       <c r="Q14" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M15" s="7"/>
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
       <c r="P15" s="7"/>
       <c r="Q15" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M16" s="7"/>
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
       <c r="P16" s="7"/>
       <c r="Q16" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="13:17" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="13:17" x14ac:dyDescent="0.25">
       <c r="M17" s="7"/>
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
       <c r="P17" s="7"/>
       <c r="Q17" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="13:17" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="13:17" x14ac:dyDescent="0.25">
       <c r="M18" s="7"/>
       <c r="N18" s="7"/>
       <c r="O18" s="7"/>
       <c r="P18" s="7"/>
       <c r="Q18" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -965,7 +968,7 @@
     <mergeCell ref="E1:K1"/>
     <mergeCell ref="M2:Q2"/>
   </mergeCells>
-  <dataValidations count="5">
+  <dataValidations disablePrompts="1" count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3" xr:uid="{B4A198EE-2B94-4E69-ABB3-F1820B4B809E}">
       <formula1>$P$3:$P$4</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
add send veps mail
</commit_message>
<xml_diff>
--- a/data/INPUT_DATOS_VEPS.xlsx
+++ b/data/INPUT_DATOS_VEPS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glorenzo\Python\VepsAutonomosPython\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA19CCD-730D-450C-8132-D1C75A0D4BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25C7046-B4E2-4AB1-B7F8-F16CFED52440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
     <author>WNS</author>
   </authors>
   <commentList>
-    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{07A28FC3-63AA-4BFA-B488-9E2C6D0305D8}">
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{07A28FC3-63AA-4BFA-B488-9E2C6D0305D8}">
       <text>
         <r>
           <rPr>
@@ -56,7 +56,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{EECF3488-78DE-4BCA-ACAC-1494A88E9DB8}">
+    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{EECF3488-78DE-4BCA-ACAC-1494A88E9DB8}">
       <text>
         <r>
           <rPr>
@@ -81,7 +81,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{BC8018FE-B940-4EA1-9195-C86B8E577E04}">
+    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{BC8018FE-B940-4EA1-9195-C86B8E577E04}">
       <text>
         <r>
           <rPr>
@@ -107,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{C4ADBE01-19FF-47B0-8ED9-4733C2F6518B}">
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{C4ADBE01-19FF-47B0-8ED9-4733C2F6518B}">
       <text>
         <r>
           <rPr>
@@ -133,7 +133,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{06F3F774-72CA-4E35-AB61-617D0715644C}">
+    <comment ref="I4" authorId="0" shapeId="0" xr:uid="{06F3F774-72CA-4E35-AB61-617D0715644C}">
       <text>
         <r>
           <rPr>
@@ -158,7 +158,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I4" authorId="0" shapeId="0" xr:uid="{6FCB2465-AD08-42C0-B19F-54EA953F5E47}">
+    <comment ref="J4" authorId="0" shapeId="0" xr:uid="{6FCB2465-AD08-42C0-B19F-54EA953F5E47}">
       <text>
         <r>
           <rPr>
@@ -189,7 +189,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="54">
   <si>
     <t>Credenciales Acceso</t>
   </si>
@@ -342,13 +342,22 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Enviar Mail?</t>
+  </si>
+  <si>
+    <t>MailCliente</t>
+  </si>
+  <si>
+    <t>lorenzogian97@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -376,6 +385,14 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -504,10 +521,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -534,6 +552,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -555,11 +582,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -838,10 +863,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R18"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,42 +875,45 @@
     <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="47.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.7109375" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" customWidth="1"/>
-    <col min="14" max="15" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="60.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="53.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="60.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="47.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.7109375" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="14.28515625" customWidth="1"/>
+    <col min="16" max="17" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="60.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="53.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="14" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="11" t="s">
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="17"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="10"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -899,39 +927,45 @@
         <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="8"/>
-      <c r="N2" s="12" t="s">
+      <c r="N2" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="O2" s="8"/>
+      <c r="P2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>20400903922</v>
       </c>
@@ -944,47 +978,53 @@
       <c r="D3" s="6">
         <v>20400903922</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="I3" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="K3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="L3" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="L3" s="7" t="s">
-        <v>50</v>
+      <c r="M3" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="N3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="P3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="Q3" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="R3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="Q3" s="7" t="s">
+      <c r="S3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="R3" s="7" t="s">
+      <c r="T3" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>20400903922</v>
       </c>
@@ -997,223 +1037,235 @@
       <c r="D4" s="6">
         <v>20400903922</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="I4" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="J4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="K4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="L4" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="L4" s="7" t="s">
-        <v>19</v>
+      <c r="M4" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="N4" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="P4" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="O4" s="7" t="s">
+      <c r="Q4" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="P4" s="7" t="s">
+      <c r="R4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="Q4" s="7" t="s">
+      <c r="S4" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="R4" s="7" t="s">
+      <c r="T4" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="H5" s="8"/>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
-      <c r="N5" s="7" t="s">
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="O5" s="7" t="s">
+      <c r="Q5" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="P5" s="7" t="s">
+      <c r="R5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7" t="s">
+      <c r="S5" s="7"/>
+      <c r="T5" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="H6" s="8"/>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7" t="s">
-        <v>48</v>
-      </c>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
       <c r="R6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7" t="s">
-        <v>49</v>
-      </c>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
       <c r="R7" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="P8" s="7"/>
       <c r="Q8" s="7"/>
-      <c r="R8" s="7" t="s">
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="P9" s="7"/>
       <c r="Q9" s="7"/>
-      <c r="R9" s="7" t="s">
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="P10" s="7"/>
       <c r="Q10" s="7"/>
-      <c r="R10" s="7" t="s">
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="P11" s="7"/>
       <c r="Q11" s="7"/>
-      <c r="R11" s="7" t="s">
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="P12" s="7"/>
       <c r="Q12" s="7"/>
-      <c r="R12" s="7" t="s">
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="P13" s="7"/>
       <c r="Q13" s="7"/>
-      <c r="R13" s="7" t="s">
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="P14" s="7"/>
       <c r="Q14" s="7"/>
-      <c r="R14" s="7" t="s">
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="P15" s="7"/>
       <c r="Q15" s="7"/>
-      <c r="R15" s="7" t="s">
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
-      <c r="R16" s="7" t="s">
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="14:18" x14ac:dyDescent="0.25">
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
+    <row r="17" spans="16:20" x14ac:dyDescent="0.25">
       <c r="P17" s="7"/>
       <c r="Q17" s="7"/>
-      <c r="R17" s="7" t="s">
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="14:18" x14ac:dyDescent="0.25">
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
+    <row r="18" spans="16:20" x14ac:dyDescent="0.25">
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
-      <c r="R18" s="7" t="s">
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="F1:L1"/>
-    <mergeCell ref="N2:R2"/>
-    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="G1:M1"/>
+    <mergeCell ref="P2:T2"/>
+    <mergeCell ref="C1:F1"/>
   </mergeCells>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:M4" xr:uid="{B4A198EE-2B94-4E69-ABB3-F1820B4B809E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:O4" xr:uid="{B4A198EE-2B94-4E69-ABB3-F1820B4B809E}">
+      <formula1>$S$3:$S$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G4" xr:uid="{1828406C-6ADF-4EFC-BDB6-D0FBBB3E3F9B}">
+      <formula1>$P$3:$P$6</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4" xr:uid="{9FCB0FBF-3539-4E18-8550-A4BBAC8B3187}">
+      <formula1>$R$3:$R$6</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:L4" xr:uid="{8FF4BDC8-A03B-4B42-987A-91C2FBDF4380}">
       <formula1>$Q$3:$Q$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F4" xr:uid="{1828406C-6ADF-4EFC-BDB6-D0FBBB3E3F9B}">
-      <formula1>$N$3:$N$6</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K4" xr:uid="{61D9AF06-4B36-4C57-9D8C-FB38695A95DC}">
+      <formula1>$T$3:$T$19</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4" xr:uid="{9FCB0FBF-3539-4E18-8550-A4BBAC8B3187}">
-      <formula1>$P$3:$P$6</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K4" xr:uid="{8FF4BDC8-A03B-4B42-987A-91C2FBDF4380}">
-      <formula1>$O$3:$O$4</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J4" xr:uid="{61D9AF06-4B36-4C57-9D8C-FB38695A95DC}">
-      <formula1>$R$3:$R$19</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3" xr:uid="{459B6677-C402-4E4C-9EC2-366A801685CF}">
-      <formula1>$P$3:$P$18</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3" xr:uid="{459B6677-C402-4E4C-9EC2-366A801685CF}">
+      <formula1>$R$3:$R$18</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{76718D7C-B896-4E81-A238-A8690DBF52C3}"/>
+    <hyperlink ref="E4" r:id="rId2" xr:uid="{07800DFE-A464-45D5-930A-C715B38A267B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>